<commit_message>
pdf functionality has been added
</commit_message>
<xml_diff>
--- a/templates/BoatsOnOrderTemplateClemens.xlsx
+++ b/templates/BoatsOnOrderTemplateClemens.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fredw\AppData\Local\Temp\scp58447\home\fwarren\.venv\smartsheet_boats_on_order\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\opt\smartsheet_boats_on_order\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -199,7 +199,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
@@ -242,6 +242,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -597,7 +600,7 @@
     <tabColor rgb="FF00B0F0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:O2000"/>
+  <dimension ref="A1:M2000"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
@@ -673,7 +676,7 @@
       <c r="E5" s="19"/>
       <c r="F5" s="19"/>
       <c r="G5" s="19"/>
-      <c r="H5" s="16"/>
+      <c r="H5" s="20"/>
       <c r="I5" s="16"/>
     </row>
     <row r="6" spans="1:9" ht="12" x14ac:dyDescent="0.2">

</xml_diff>